<commit_message>
Web Scraper added to find Jobs
</commit_message>
<xml_diff>
--- a/data/Mentee_Data.xlsx
+++ b/data/Mentee_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Admin/Desktop/MyDocs/QMentoring algo/Mentor-Matching-Algo/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19EAA13D-121F-374B-958D-D9E6BF3C9D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{978D8352-74F8-7148-8400-B824C7C641AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="78">
   <si>
     <t>ID</t>
   </si>
@@ -171,6 +171,93 @@
   </si>
   <si>
     <t>Carter</t>
+  </si>
+  <si>
+    <t>BA FT Drama</t>
+  </si>
+  <si>
+    <t>BSc FT Chemistry</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>13242R455</t>
+  </si>
+  <si>
+    <t>School of X</t>
+  </si>
+  <si>
+    <t>School of Y</t>
+  </si>
+  <si>
+    <t>School of S</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Speaks Urdu, interested in programming</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>Software Engineering or Programming, Cyber Security</t>
+  </si>
+  <si>
+    <t>BSc FT Computer Science</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>English or writer</t>
+  </si>
+  <si>
+    <t>chemist, pharmasist</t>
+  </si>
+  <si>
+    <t>scientist, researcher, biologist</t>
+  </si>
+  <si>
+    <t>No Preference</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Option 1 - A mentor who studied the same degree as me but works in any industry/job role</t>
+  </si>
+  <si>
+    <t>Option 2 - A mentor who works in the industry/job role that I am interested in</t>
+  </si>
+  <si>
+    <t>Option 3 - A mentor who can support with entrepreneurship</t>
+  </si>
+  <si>
+    <t>Stage 1 - I am looking to explore entrepreneurship</t>
+  </si>
+  <si>
+    <t>Stage 3 - I am a current entrepreneur in need extra support with my business</t>
+  </si>
+  <si>
+    <t>Planning for the future and goal setting, Gaining insight to an industry/profession, Building a professional network, Writing/improving CVs, job applications and covering letters</t>
+  </si>
+  <si>
+    <t>Interview practice and preparation, Finding work experience (shadowing/internships/part-time work), Developing entrepreneurial skills, Support with setting up or growing a business</t>
+  </si>
+  <si>
+    <t>Support with setting up or growing a business, Planning for the future and goal setting, Building a professional network</t>
   </si>
 </sst>
 </file>
@@ -528,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AQ4"/>
+  <dimension ref="A1:AQ5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="AM1" zoomScale="119" workbookViewId="0">
+      <selection activeCell="AM4" sqref="AM4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -723,6 +810,33 @@
       <c r="G2" s="1">
         <v>200100227</v>
       </c>
+      <c r="I2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AN2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AP2" s="1" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="3" spans="1:43" x14ac:dyDescent="0.2">
       <c r="D3" s="1" t="s">
@@ -734,6 +848,33 @@
       <c r="G3" s="1">
         <v>220102345</v>
       </c>
+      <c r="I3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AN3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AP3" s="1" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="4" spans="1:43" x14ac:dyDescent="0.2">
       <c r="D4" s="1" t="s">
@@ -744,6 +885,74 @@
       </c>
       <c r="G4" s="1">
         <v>190101089</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AN4" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AO4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AP4" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="D5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AI5" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AN5" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AO5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AP5" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>